<commit_message>
Fixes 1 on TC32
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\LogixalQA\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B47752-CEFD-406B-A9C2-B768772C1FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD9045A-E4AD-4383-860A-B02F5EA837CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>TestCase</t>
   </si>
@@ -590,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -897,7 +897,7 @@
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
       <c r="B24" s="5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>48</v>
@@ -905,24 +905,22 @@
       <c r="D24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>48</v>
+      <c r="E24" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3"/>
@@ -930,25 +928,12 @@
         <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="3"/>
-      <c r="B27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1089,21 +1074,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1300,24 +1270,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1334,4 +1302,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixes 2 on TC32
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\LogixalQA\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD9045A-E4AD-4383-860A-B02F5EA837CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F394E-75B4-4A19-B57C-13777A11803C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>TestCase</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>ContactMenu</t>
-  </si>
-  <si>
-    <t>VERIFY_TEXT_PRESENT</t>
   </si>
   <si>
     <t>Storelocator</t>
@@ -590,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -638,16 +635,16 @@
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
@@ -662,16 +659,16 @@
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
@@ -695,13 +692,13 @@
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5"/>
     </row>
@@ -711,10 +708,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="5"/>
     </row>
@@ -727,7 +724,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -742,7 +739,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>15</v>
@@ -754,10 +751,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -779,7 +776,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -801,7 +798,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -811,40 +808,40 @@
         <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -854,13 +851,13 @@
         <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -869,10 +866,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="3"/>
     </row>
@@ -897,17 +894,15 @@
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
       <c r="B24" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3"/>
@@ -918,22 +913,9 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="3"/>
-      <c r="B26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -969,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -977,7 +959,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -985,12 +967,12 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="5" t="b">
         <v>1</v>
@@ -998,7 +980,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="b">
         <v>1</v>
@@ -1006,7 +988,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3">
         <v>10010</v>
@@ -1014,47 +996,47 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="3" t="b">
         <v>1</v>
@@ -1062,10 +1044,10 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>